<commit_message>
Switched to 32-bit, screenshot seems to work, triple-buffering to avoid hiccups
</commit_message>
<xml_diff>
--- a/DMHelper/src/release notes/Release Checklist v2.4.xlsx
+++ b/DMHelper/src/release notes/Release Checklist v2.4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218A9E83-26A9-4F96-81D7-D55B65A8ED22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E972D5E3-852C-4A7F-8379-E8F9CD21B0A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -639,7 +639,7 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -672,7 +672,7 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -713,7 +713,7 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -724,7 +724,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -735,7 +735,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>